<commit_message>
changed percents to numbers
</commit_message>
<xml_diff>
--- a/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-07-29-Spawning-Calculations.xlsx
+++ b/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-07-29-Spawning-Calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sex" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="194">
   <si>
     <t>Sex</t>
   </si>
@@ -627,6 +627,15 @@
   <si>
     <t>Amount Male Added (mL)</t>
   </si>
+  <si>
+    <t>22 total low females</t>
+  </si>
+  <si>
+    <t>26 total ambient females</t>
+  </si>
+  <si>
+    <t>6 total heat shock females</t>
+  </si>
 </sst>
 </file>
 
@@ -750,7 +759,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -782,6 +791,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1785,7 +1795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD62"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18395,6 +18407,9 @@
       <c r="B25">
         <v>1</v>
       </c>
+      <c r="C25" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -18659,6 +18674,9 @@
       <c r="B55">
         <v>1</v>
       </c>
+      <c r="C55" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
@@ -18723,6 +18741,9 @@
       </c>
       <c r="B62">
         <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -18735,7 +18756,7 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20880,8 +20901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20983,7 +21004,7 @@
         <f>(K2*J2)/E2</f>
         <v>71200</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="19">
         <f>L2/C2</f>
         <v>0.33904761904762076</v>
       </c>
@@ -21029,7 +21050,7 @@
         <f>(K3*J3)/E3</f>
         <v>98933.333333333343</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M3" s="19">
         <f t="shared" ref="M3:M27" si="3">L3/C3</f>
         <v>0.47111111111111353</v>
       </c>
@@ -21075,7 +21096,7 @@
         <f>(K4*J4)/E4</f>
         <v>107280</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="19">
         <f t="shared" si="3"/>
         <v>0.51085714285714545</v>
       </c>
@@ -21121,7 +21142,7 @@
         <f t="shared" ref="L5:L27" si="4">(K5*J5)/E5</f>
         <v>88500</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="19">
         <f t="shared" si="3"/>
         <v>0.42142857142857354</v>
       </c>
@@ -21167,7 +21188,7 @@
         <f t="shared" si="4"/>
         <v>85333.333333333343</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="19">
         <f t="shared" si="3"/>
         <v>0.4063492063492084</v>
       </c>
@@ -21213,7 +21234,7 @@
         <f t="shared" si="4"/>
         <v>65079.365079365074</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="19">
         <f t="shared" si="3"/>
         <v>0.30990173847316854</v>
       </c>
@@ -21259,7 +21280,7 @@
         <f t="shared" si="4"/>
         <v>93866.666666666672</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="19">
         <f t="shared" si="3"/>
         <v>0.44698412698412926</v>
       </c>
@@ -21305,7 +21326,7 @@
         <f t="shared" si="4"/>
         <v>67200</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="19">
         <f t="shared" si="3"/>
         <v>0.32000000000000162</v>
       </c>
@@ -21351,7 +21372,7 @@
         <f t="shared" si="4"/>
         <v>100520</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="19">
         <f t="shared" si="3"/>
         <v>0.47866666666666907</v>
       </c>
@@ -21397,7 +21418,7 @@
         <f t="shared" si="4"/>
         <v>37777.777777777774</v>
       </c>
-      <c r="M11" s="17">
+      <c r="M11" s="19">
         <f t="shared" si="3"/>
         <v>0.17989417989418077</v>
       </c>
@@ -21443,7 +21464,7 @@
         <f t="shared" si="4"/>
         <v>136800</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="19">
         <f t="shared" si="3"/>
         <v>0.65142857142857469</v>
       </c>
@@ -21489,7 +21510,7 @@
         <f t="shared" si="4"/>
         <v>79733.333333333343</v>
       </c>
-      <c r="M13" s="17">
+      <c r="M13" s="19">
         <f t="shared" si="3"/>
         <v>0.37968253968254162</v>
       </c>
@@ -21537,7 +21558,7 @@
         <f t="shared" si="4"/>
         <v>107240</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="19">
         <f t="shared" si="3"/>
         <v>0.51066666661455828</v>
       </c>
@@ -21586,7 +21607,7 @@
         <f t="shared" si="4"/>
         <v>72727.272727272721</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="19">
         <f t="shared" si="3"/>
         <v>0.3463203462850078</v>
       </c>
@@ -21632,7 +21653,7 @@
         <f t="shared" si="4"/>
         <v>212666.66666666666</v>
       </c>
-      <c r="M16" s="17">
+      <c r="M16" s="19">
         <f t="shared" si="3"/>
         <v>1.0126984125950769</v>
       </c>
@@ -21681,7 +21702,7 @@
         <f t="shared" si="4"/>
         <v>122320</v>
       </c>
-      <c r="M17" s="17">
+      <c r="M17" s="19">
         <f t="shared" si="3"/>
         <v>0.58247619041675458</v>
       </c>
@@ -21727,7 +21748,7 @@
         <f t="shared" si="4"/>
         <v>116160</v>
       </c>
-      <c r="M18" s="17">
+      <c r="M18" s="19">
         <f t="shared" si="3"/>
         <v>0.55314285708641442</v>
       </c>
@@ -21773,7 +21794,7 @@
         <f t="shared" si="4"/>
         <v>208800</v>
       </c>
-      <c r="M19" s="17">
+      <c r="M19" s="19">
         <f t="shared" si="3"/>
         <v>0.99428571418425737</v>
       </c>
@@ -21822,7 +21843,7 @@
         <f t="shared" si="4"/>
         <v>129066.66666666667</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="19">
         <f t="shared" si="3"/>
         <v>0.61460317454046054</v>
       </c>
@@ -21868,7 +21889,7 @@
         <f t="shared" si="4"/>
         <v>152720</v>
       </c>
-      <c r="M21" s="17">
+      <c r="M21" s="19">
         <f t="shared" si="3"/>
         <v>0.72723809516388793</v>
       </c>
@@ -21914,7 +21935,7 @@
         <f t="shared" si="4"/>
         <v>111733.33333333333</v>
       </c>
-      <c r="M22" s="17">
+      <c r="M22" s="19">
         <f t="shared" si="3"/>
         <v>0.53206349200920033</v>
       </c>
@@ -21960,7 +21981,7 @@
         <f t="shared" si="4"/>
         <v>90666.666666666657</v>
       </c>
-      <c r="M23" s="17">
+      <c r="M23" s="19">
         <f t="shared" si="3"/>
         <v>0.43174603170197634</v>
       </c>
@@ -22006,7 +22027,7 @@
         <f t="shared" si="4"/>
         <v>112800</v>
       </c>
-      <c r="M24" s="17">
+      <c r="M24" s="19">
         <f t="shared" si="3"/>
         <v>0.5371428570880471</v>
       </c>
@@ -22052,7 +22073,7 @@
         <f t="shared" si="4"/>
         <v>244333.33333333337</v>
       </c>
-      <c r="M25" s="17">
+      <c r="M25" s="19">
         <f t="shared" si="3"/>
         <v>1.163492063373341</v>
       </c>
@@ -22101,7 +22122,7 @@
         <f t="shared" si="4"/>
         <v>498666.66666666674</v>
       </c>
-      <c r="M26" s="17">
+      <c r="M26" s="19">
         <f t="shared" si="3"/>
         <v>0.80736507936507873</v>
       </c>
@@ -22147,7 +22168,7 @@
         <f t="shared" si="4"/>
         <v>352000</v>
       </c>
-      <c r="M27" s="17">
+      <c r="M27" s="19">
         <f t="shared" si="3"/>
         <v>0.56990476190476136</v>
       </c>
@@ -22179,7 +22200,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="102" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22423,7 +22444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added number of females used to pools
</commit_message>
<xml_diff>
--- a/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-07-29-Spawning-Calculations.xlsx
+++ b/data/Manchester/2017-07-30-Pacific-Oyster-Larvae/2017-07-29-Spawning-Calculations.xlsx
@@ -759,7 +759,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -791,7 +791,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="25" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -20902,7 +20901,7 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21004,7 +21003,7 @@
         <f>(K2*J2)/E2</f>
         <v>71200</v>
       </c>
-      <c r="M2" s="19">
+      <c r="M2" s="17">
         <f>L2/C2</f>
         <v>0.33904761904762076</v>
       </c>
@@ -21050,7 +21049,7 @@
         <f>(K3*J3)/E3</f>
         <v>98933.333333333343</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="17">
         <f t="shared" ref="M3:M27" si="3">L3/C3</f>
         <v>0.47111111111111353</v>
       </c>
@@ -21096,7 +21095,7 @@
         <f>(K4*J4)/E4</f>
         <v>107280</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="17">
         <f t="shared" si="3"/>
         <v>0.51085714285714545</v>
       </c>
@@ -21142,7 +21141,7 @@
         <f t="shared" ref="L5:L27" si="4">(K5*J5)/E5</f>
         <v>88500</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="17">
         <f t="shared" si="3"/>
         <v>0.42142857142857354</v>
       </c>
@@ -21188,7 +21187,7 @@
         <f t="shared" si="4"/>
         <v>85333.333333333343</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="17">
         <f t="shared" si="3"/>
         <v>0.4063492063492084</v>
       </c>
@@ -21234,7 +21233,7 @@
         <f t="shared" si="4"/>
         <v>65079.365079365074</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="17">
         <f t="shared" si="3"/>
         <v>0.30990173847316854</v>
       </c>
@@ -21280,7 +21279,7 @@
         <f t="shared" si="4"/>
         <v>93866.666666666672</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="17">
         <f t="shared" si="3"/>
         <v>0.44698412698412926</v>
       </c>
@@ -21326,7 +21325,7 @@
         <f t="shared" si="4"/>
         <v>67200</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="17">
         <f t="shared" si="3"/>
         <v>0.32000000000000162</v>
       </c>
@@ -21372,7 +21371,7 @@
         <f t="shared" si="4"/>
         <v>100520</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="17">
         <f t="shared" si="3"/>
         <v>0.47866666666666907</v>
       </c>
@@ -21418,7 +21417,7 @@
         <f t="shared" si="4"/>
         <v>37777.777777777774</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="17">
         <f t="shared" si="3"/>
         <v>0.17989417989418077</v>
       </c>
@@ -21464,7 +21463,7 @@
         <f t="shared" si="4"/>
         <v>136800</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="17">
         <f t="shared" si="3"/>
         <v>0.65142857142857469</v>
       </c>
@@ -21510,7 +21509,7 @@
         <f t="shared" si="4"/>
         <v>79733.333333333343</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="17">
         <f t="shared" si="3"/>
         <v>0.37968253968254162</v>
       </c>
@@ -21558,7 +21557,7 @@
         <f t="shared" si="4"/>
         <v>107240</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="17">
         <f t="shared" si="3"/>
         <v>0.51066666661455828</v>
       </c>
@@ -21607,7 +21606,7 @@
         <f t="shared" si="4"/>
         <v>72727.272727272721</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="17">
         <f t="shared" si="3"/>
         <v>0.3463203462850078</v>
       </c>
@@ -21653,7 +21652,7 @@
         <f t="shared" si="4"/>
         <v>212666.66666666666</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="17">
         <f t="shared" si="3"/>
         <v>1.0126984125950769</v>
       </c>
@@ -21702,7 +21701,7 @@
         <f t="shared" si="4"/>
         <v>122320</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="17">
         <f t="shared" si="3"/>
         <v>0.58247619041675458</v>
       </c>
@@ -21748,7 +21747,7 @@
         <f t="shared" si="4"/>
         <v>116160</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="17">
         <f t="shared" si="3"/>
         <v>0.55314285708641442</v>
       </c>
@@ -21794,7 +21793,7 @@
         <f t="shared" si="4"/>
         <v>208800</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="17">
         <f t="shared" si="3"/>
         <v>0.99428571418425737</v>
       </c>
@@ -21843,7 +21842,7 @@
         <f t="shared" si="4"/>
         <v>129066.66666666667</v>
       </c>
-      <c r="M20" s="19">
+      <c r="M20" s="17">
         <f t="shared" si="3"/>
         <v>0.61460317454046054</v>
       </c>
@@ -21889,7 +21888,7 @@
         <f t="shared" si="4"/>
         <v>152720</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="17">
         <f t="shared" si="3"/>
         <v>0.72723809516388793</v>
       </c>
@@ -21935,7 +21934,7 @@
         <f t="shared" si="4"/>
         <v>111733.33333333333</v>
       </c>
-      <c r="M22" s="19">
+      <c r="M22" s="17">
         <f t="shared" si="3"/>
         <v>0.53206349200920033</v>
       </c>
@@ -21981,7 +21980,7 @@
         <f t="shared" si="4"/>
         <v>90666.666666666657</v>
       </c>
-      <c r="M23" s="19">
+      <c r="M23" s="17">
         <f t="shared" si="3"/>
         <v>0.43174603170197634</v>
       </c>
@@ -22027,7 +22026,7 @@
         <f t="shared" si="4"/>
         <v>112800</v>
       </c>
-      <c r="M24" s="19">
+      <c r="M24" s="17">
         <f t="shared" si="3"/>
         <v>0.5371428570880471</v>
       </c>
@@ -22073,7 +22072,7 @@
         <f t="shared" si="4"/>
         <v>244333.33333333337</v>
       </c>
-      <c r="M25" s="19">
+      <c r="M25" s="17">
         <f t="shared" si="3"/>
         <v>1.163492063373341</v>
       </c>
@@ -22122,7 +22121,7 @@
         <f t="shared" si="4"/>
         <v>498666.66666666674</v>
       </c>
-      <c r="M26" s="19">
+      <c r="M26" s="17">
         <f t="shared" si="3"/>
         <v>0.80736507936507873</v>
       </c>
@@ -22168,7 +22167,7 @@
         <f t="shared" si="4"/>
         <v>352000</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="17">
         <f t="shared" si="3"/>
         <v>0.56990476190476136</v>
       </c>

</xml_diff>